<commit_message>
ajustado bug do grafico e atualização do profile
</commit_message>
<xml_diff>
--- a/my-life-dashboard/public/TabelaExemplo.xlsx
+++ b/my-life-dashboard/public/TabelaExemplo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trabalho\ProjetosPessoais\myLifeDashboard\my-life-dashboard\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81BF87E-8B69-4038-A58E-B7BB3E69E019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2B3948-6A4F-4316-B230-BD20498905C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{069C4872-7557-412F-975C-5ACDED8D0BCC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="56">
   <si>
     <t>Data</t>
   </si>
@@ -100,6 +100,108 @@
   </si>
   <si>
     <t>Celular 5/8</t>
+  </si>
+  <si>
+    <t>borges lanche</t>
+  </si>
+  <si>
+    <t>vila dionisio</t>
+  </si>
+  <si>
+    <t>Uber</t>
+  </si>
+  <si>
+    <t>indo pro vila</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>ifood</t>
+  </si>
+  <si>
+    <t>sorvete</t>
+  </si>
+  <si>
+    <t>lanche</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>voltando pra casa</t>
+  </si>
+  <si>
+    <t>fabrica</t>
+  </si>
+  <si>
+    <t>indo fabrica</t>
+  </si>
+  <si>
+    <t>Faculdade</t>
+  </si>
+  <si>
+    <t>FATEC inscrição</t>
+  </si>
+  <si>
+    <t>cupom</t>
+  </si>
+  <si>
+    <t>Farmacia</t>
+  </si>
+  <si>
+    <t>remedio queimação</t>
+  </si>
+  <si>
+    <t>Supermercado</t>
+  </si>
+  <si>
+    <t>salgadin</t>
+  </si>
+  <si>
+    <t>Galpao 20</t>
+  </si>
+  <si>
+    <t>Academia</t>
+  </si>
+  <si>
+    <t>Academia 7/11</t>
+  </si>
+  <si>
+    <t>Seu site</t>
+  </si>
+  <si>
+    <t>AME</t>
+  </si>
+  <si>
+    <t>celular 6/8</t>
+  </si>
+  <si>
+    <t>MercadoLivre</t>
+  </si>
+  <si>
+    <t>god of war 7/10</t>
+  </si>
+  <si>
+    <t>Jogos</t>
+  </si>
+  <si>
+    <t>lanche pra sobrinha</t>
+  </si>
+  <si>
+    <t>HBO Max</t>
+  </si>
+  <si>
+    <t>Netflix</t>
+  </si>
+  <si>
+    <t>armazem baixada</t>
+  </si>
+  <si>
+    <t>BurgerKing</t>
+  </si>
+  <si>
+    <t>lanchinho</t>
   </si>
 </sst>
 </file>
@@ -135,9 +237,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -160,8 +263,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BC12DB74-FFEB-49F3-AF43-359AD1F5FB1B}" name="Tabela1" displayName="Tabela1" ref="A1:F7" totalsRowShown="0">
-  <autoFilter ref="A1:F7" xr:uid="{BC12DB74-FFEB-49F3-AF43-359AD1F5FB1B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BC12DB74-FFEB-49F3-AF43-359AD1F5FB1B}" name="Tabela1" displayName="Tabela1" ref="A1:F47" totalsRowShown="0">
+  <autoFilter ref="A1:F47" xr:uid="{BC12DB74-FFEB-49F3-AF43-359AD1F5FB1B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F7">
     <sortCondition descending="1" ref="A1:A7"/>
   </sortState>
@@ -474,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A38F936-F46C-4266-BB96-243ABC31C6A7}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,6 +733,806 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45066</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45066</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>87.7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45066</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10">
+        <v>16.93</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45065</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>19.739999999999998</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45065</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>22.25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45064</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>14.9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45060</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <v>22.24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45059</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15">
+        <v>14.18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45059</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45059</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45059</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45059</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45059</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20">
+        <v>10.62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45058</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21">
+        <v>22.25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45054</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22">
+        <v>91</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45053</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <v>22.23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45053</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <v>13.31</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45053</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25">
+        <v>46</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>45053</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <v>32.54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28">
+        <v>14</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29">
+        <v>34.9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30">
+        <v>12</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31">
+        <v>99</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32">
+        <v>19.329999999999998</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <v>14</v>
+      </c>
+      <c r="F33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <v>20</v>
+      </c>
+      <c r="F34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35">
+        <v>289.74</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="2">
+        <v>32.9</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>45011</v>
+      </c>
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37">
+        <v>14.99</v>
+      </c>
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <v>52.79</v>
+      </c>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>45010</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39">
+        <v>13.95</v>
+      </c>
+      <c r="F39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>45009</v>
+      </c>
+      <c r="B40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40">
+        <v>55.9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>45008</v>
+      </c>
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41">
+        <v>21.24</v>
+      </c>
+      <c r="F41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>45004</v>
+      </c>
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42">
+        <v>21.2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>45003</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43">
+        <v>10</v>
+      </c>
+      <c r="F43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>45003</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44">
+        <v>12</v>
+      </c>
+      <c r="F44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>45003</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45">
+        <v>15</v>
+      </c>
+      <c r="F45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45002</v>
+      </c>
+      <c r="B46" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46">
+        <v>14.9</v>
+      </c>
+      <c r="F46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>45002</v>
+      </c>
+      <c r="B47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="F47" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>